<commit_message>
update report in kmeans
</commit_message>
<xml_diff>
--- a/clustering/Bookof5year.xlsx
+++ b/clustering/Bookof5year.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PPUNN\Documents\gitproject\stat_assignment2\clustering\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198CB8B5-0F70-4026-874E-3A0325D5E2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633177F6-90A6-441C-A962-595B4D0EDBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{26AC53EC-38BD-482E-9C66-EBBFDE5316FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{26AC53EC-38BD-482E-9C66-EBBFDE5316FE}"/>
   </bookViews>
   <sheets>
     <sheet name="2560" sheetId="2" r:id="rId1"/>
@@ -271,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -300,6 +300,7 @@
     <xf numFmtId="4" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="4" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="2" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -621,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0656744-F332-426A-AAC5-9276B77DAB9A}">
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection sqref="A1:H21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" x14ac:dyDescent="0.55000000000000004"/>
@@ -1326,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551A7F79-D4A1-43B6-8092-6A0C6200F037}">
   <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:H30"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1906,26 +1907,26 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="24" t="s">
         <v>1</v>
       </c>
       <c r="C26" s="14">
-        <v>3218.8692310000001</v>
+        <v>3242.1153850000001</v>
       </c>
       <c r="D26" s="14">
-        <v>258020.8</v>
+        <v>250754.5</v>
       </c>
       <c r="E26" s="14">
-        <v>12014.6</v>
+        <v>69232.600000000006</v>
       </c>
       <c r="F26" s="14">
-        <v>68291.133333000005</v>
+        <v>12235.8</v>
       </c>
       <c r="G26" s="14">
-        <v>9248.9</v>
+        <v>17815</v>
       </c>
       <c r="H26" s="14">
-        <v>17293.900000000001</v>
+        <v>9492.6</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
@@ -1933,22 +1934,22 @@
         <v>2</v>
       </c>
       <c r="C27" s="14">
-        <v>2494.7307689999998</v>
+        <v>2428.792308</v>
       </c>
       <c r="D27" s="14">
-        <v>36824.800000000003</v>
+        <v>33148.800000000003</v>
       </c>
       <c r="E27" s="14">
-        <v>6188.9</v>
+        <v>18229.400000000001</v>
       </c>
       <c r="F27" s="14">
-        <v>18122.833332999999</v>
+        <v>6177.6</v>
       </c>
       <c r="G27" s="14">
-        <v>2344.5</v>
+        <v>14050.7</v>
       </c>
       <c r="H27" s="14">
-        <v>12809.2</v>
+        <v>2308.9</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
@@ -1956,22 +1957,22 @@
         <v>3</v>
       </c>
       <c r="C28" s="14">
-        <v>2256</v>
+        <v>2395.461538</v>
       </c>
       <c r="D28" s="14">
-        <v>33810.300000000003</v>
+        <v>34287.599999999999</v>
       </c>
       <c r="E28" s="14">
-        <v>3343.7</v>
+        <v>28952.166667000001</v>
       </c>
       <c r="F28" s="14">
-        <v>24957.133333000002</v>
+        <v>3177.1</v>
       </c>
       <c r="G28" s="14">
-        <v>137892.70000000001</v>
+        <v>29648.7</v>
       </c>
       <c r="H28" s="14">
-        <v>29055.5</v>
+        <v>156059.29999999999</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
@@ -1979,22 +1980,22 @@
         <v>4</v>
       </c>
       <c r="C29" s="14">
-        <v>5629.7846149999996</v>
+        <v>6189.2846149999996</v>
       </c>
       <c r="D29" s="14">
-        <v>175509.7</v>
+        <v>180797.9</v>
       </c>
       <c r="E29" s="14">
-        <v>238.8</v>
+        <v>5576.1666670000004</v>
       </c>
       <c r="F29" s="14">
-        <v>4094.1333330000002</v>
+        <v>89.2</v>
       </c>
       <c r="G29" s="14">
-        <v>462.3</v>
+        <v>264311.40000000002</v>
       </c>
       <c r="H29" s="14">
-        <v>246083.20000000001</v>
+        <v>268.39999999999998</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="24" x14ac:dyDescent="0.55000000000000004">
@@ -2002,26 +2003,27 @@
         <v>5</v>
       </c>
       <c r="C30" s="14">
-        <v>2409.9538459999999</v>
+        <v>2217.707692</v>
       </c>
       <c r="D30" s="14">
-        <v>9244.4</v>
+        <v>8958.9</v>
       </c>
       <c r="E30" s="14">
-        <v>195927.6</v>
+        <v>29759.133333000002</v>
       </c>
       <c r="F30" s="14">
-        <v>28695.3</v>
+        <v>216561.9</v>
       </c>
       <c r="G30" s="14">
-        <v>801.6</v>
+        <v>28477.8</v>
       </c>
       <c r="H30" s="14">
-        <v>27566.7</v>
+        <v>638.79999999999995</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2733,8 +2735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F0DB6E5-9B27-4022-9BF8-C5211760437F}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24:G29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24" x14ac:dyDescent="0.55000000000000004"/>
@@ -3314,19 +3316,19 @@
       <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="14">
         <v>4312.8615380000001</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="14">
         <v>140597</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="14">
         <v>17195.400000000001</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="14">
         <v>19158.099999999999</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="14">
         <v>13093.2</v>
       </c>
     </row>
@@ -3334,19 +3336,19 @@
       <c r="B26" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="14">
         <v>2523.9923079999999</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="14">
         <v>19828.599999999999</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="14">
         <v>8126.15</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="14">
         <v>13538</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="14">
         <v>6734.3</v>
       </c>
     </row>
@@ -3354,19 +3356,19 @@
       <c r="B27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="14">
         <v>3007.853846</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="14">
         <v>18475.466667000001</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="14">
         <v>116851.35</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="14">
         <v>34694.800000000003</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="14">
         <v>3108.5</v>
       </c>
     </row>
@@ -3374,19 +3376,19 @@
       <c r="B28" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="14">
         <v>14809.292308</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="14">
         <v>33808.300000000003</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="14">
         <v>1379.95</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="14">
         <v>256160.3</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="14">
         <v>873.7</v>
       </c>
     </row>
@@ -3394,19 +3396,19 @@
       <c r="B29" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="14">
         <v>2424.8384620000002</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="14">
         <v>34205.133332999998</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="14">
         <v>784.05</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="14">
         <v>29456.2</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="14">
         <v>225866.3</v>
       </c>
     </row>
@@ -3419,7 +3421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A45196C-3ACF-4496-AB2C-6356CB4164C7}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B26" sqref="B26:G31"/>
     </sheetView>
   </sheetViews>

</xml_diff>